<commit_message>
Changes for new season, preseason data now workable
</commit_message>
<xml_diff>
--- a/Data/Logos.xlsx
+++ b/Data/Logos.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="qiaYlqSHv/Xp1uFCzmmSQ+LStCSll70P7qHEw0vFDi4="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="FLZyQrvu4hXTxhi2hKNmLt31ZxkiVPhR5jjScUli0rM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="1046">
   <si>
     <t>TEAM</t>
   </si>
@@ -1749,6 +1749,12 @@
     <t>https://content.sportslogos.net/logos/33/768/full/new_hampshire_wildcats_logo_primary_2021_sportslogosnet-9635.png</t>
   </si>
   <si>
+    <t>New Haven</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/New_Haven_Chargers#/media/File:New_Haven_Chargers_secondary_logo.svg</t>
+  </si>
+  <si>
     <t>New Mexico</t>
   </si>
   <si>
@@ -2475,9 +2481,6 @@
     <t>St Francis PA</t>
   </si>
   <si>
-    <t>St. Francis (PA)</t>
-  </si>
-  <si>
     <t>https://content.sportslogos.net/logos/34/821/full/saint_francis_red_flash_logo_primary_2018_sportslogosnet-7517.png</t>
   </si>
   <si>
@@ -2625,16 +2628,13 @@
     <t>https://content.sportslogos.net/logos/34/866/full/texas_a&amp;m_aggies_logo_primary_2021_sportslogosnet-5634.png</t>
   </si>
   <si>
-    <t>Texas A&amp;M Commerce</t>
+    <t>East Texas A&amp;M</t>
   </si>
   <si>
     <t>E Texas A&amp;M</t>
   </si>
   <si>
     <t>AM Commerce</t>
-  </si>
-  <si>
-    <t>East Texas A&amp;M</t>
   </si>
   <si>
     <t>https://content.sportslogos.net/logos/30/6863/full/a&amp;m-commerce_lions_logo_primary_2013_sportslogosnet-6740.png</t>
@@ -3160,7 +3160,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -3177,6 +3177,9 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <color rgb="FF0000FF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3192,7 +3195,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3204,6 +3207,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -7353,22 +7359,16 @@
       </c>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="A197" s="1" t="s">
+      <c r="A197" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="D197" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="C197" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="D197" s="1" t="s">
-        <v>577</v>
-      </c>
-      <c r="E197" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F197" s="1" t="s">
+      <c r="E197" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F197" s="5" t="s">
         <v>578</v>
       </c>
     </row>
@@ -7376,28 +7376,28 @@
       <c r="A198" s="1" t="s">
         <v>579</v>
       </c>
-      <c r="B198" s="2" t="s">
+      <c r="B198" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F198" s="1" t="s">
         <v>580</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="D198" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E198" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F198" s="1" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="199" ht="15.75" customHeight="1">
       <c r="A199" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>582</v>
       </c>
       <c r="C199" s="1" t="s">
         <v>583</v>
@@ -7406,7 +7406,7 @@
         <v>583</v>
       </c>
       <c r="E199" s="1" t="s">
-        <v>351</v>
+        <v>269</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>584</v>
@@ -7426,7 +7426,7 @@
         <v>585</v>
       </c>
       <c r="E200" s="1" t="s">
-        <v>141</v>
+        <v>351</v>
       </c>
       <c r="F200" s="1" t="s">
         <v>586</v>
@@ -7437,36 +7437,36 @@
         <v>587</v>
       </c>
       <c r="B201" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F201" s="1" t="s">
         <v>588</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="D201" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="E201" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F201" s="1" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="202" ht="15.75" customHeight="1">
       <c r="A202" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>591</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E202" s="1" t="s">
-        <v>29</v>
+        <v>351</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>592</v>
@@ -7477,27 +7477,27 @@
         <v>593</v>
       </c>
       <c r="B203" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="E203" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F203" s="1" t="s">
         <v>594</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="D203" s="1" t="s">
-        <v>595</v>
-      </c>
-      <c r="E203" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F203" s="1" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="204" ht="15.75" customHeight="1">
       <c r="A204" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C204" s="1" t="s">
         <v>597</v>
@@ -7506,27 +7506,27 @@
         <v>597</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="F204" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="205" ht="15.75" customHeight="1">
       <c r="A205" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B205" s="1" t="s">
         <v>600</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>600</v>
-      </c>
       <c r="C205" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="F205" s="1" t="s">
         <v>601</v>
@@ -7536,77 +7536,77 @@
       <c r="A206" s="1" t="s">
         <v>602</v>
       </c>
-      <c r="B206" s="1" t="s">
-        <v>603</v>
+      <c r="B206" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>602</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
       <c r="F206" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="207" ht="15.75" customHeight="1">
       <c r="A207" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="C207" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B207" s="1" t="s">
+      <c r="D207" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="E207" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F207" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="C207" s="1" t="s">
+    </row>
+    <row r="208" ht="15.75" customHeight="1">
+      <c r="A208" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="D207" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="E207" s="1" t="s">
+      <c r="B208" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="E208" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F207" s="1" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="208" ht="15.75" customHeight="1">
-      <c r="A208" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B208" s="1" t="s">
+      <c r="F208" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="C208" s="1" t="s">
+    </row>
+    <row r="209" ht="15.75" customHeight="1">
+      <c r="A209" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="D208" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="E208" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F208" s="1" t="s">
+      <c r="B209" s="1" t="s">
         <v>613</v>
-      </c>
-    </row>
-    <row r="209" ht="15.75" customHeight="1">
-      <c r="A209" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B209" s="1" t="s">
-        <v>614</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>614</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>220</v>
+        <v>92</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>615</v>
@@ -7617,76 +7617,76 @@
         <v>616</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F210" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="211" ht="15.75" customHeight="1">
       <c r="A211" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="C211" s="1" t="s">
         <v>620</v>
-      </c>
-      <c r="B211" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>622</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>620</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>67</v>
+        <v>220</v>
       </c>
       <c r="F211" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="212" ht="15.75" customHeight="1">
       <c r="A212" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>625</v>
+        <v>622</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>623</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>624</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="E212" s="1" t="s">
-        <v>159</v>
+        <v>67</v>
       </c>
       <c r="F212" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="213" ht="15.75" customHeight="1">
       <c r="A213" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>627</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E213" s="1" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F213" s="1" t="s">
         <v>628</v>
@@ -7696,8 +7696,8 @@
       <c r="A214" s="1" t="s">
         <v>629</v>
       </c>
-      <c r="B214" s="1" t="s">
-        <v>630</v>
+      <c r="B214" s="2" t="s">
+        <v>629</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>629</v>
@@ -7706,107 +7706,107 @@
         <v>629</v>
       </c>
       <c r="E214" s="1" t="s">
-        <v>255</v>
+        <v>138</v>
       </c>
       <c r="F214" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="215" ht="15.75" customHeight="1">
       <c r="A215" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="B215" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="B215" s="1" t="s">
-        <v>633</v>
-      </c>
       <c r="C215" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>255</v>
       </c>
       <c r="F215" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="216" ht="15.75" customHeight="1">
       <c r="A216" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="B216" s="1" t="s">
         <v>635</v>
       </c>
-      <c r="B216" s="1" t="s">
+      <c r="C216" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="E216" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F216" s="1" t="s">
         <v>636</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>635</v>
-      </c>
-      <c r="E216" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F216" s="1" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="217" ht="15.75" customHeight="1">
       <c r="A217" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="B217" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="B217" s="1" t="s">
+      <c r="C217" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="E217" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F217" s="1" t="s">
         <v>639</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="E217" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F217" s="1" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="218" ht="15.75" customHeight="1">
       <c r="A218" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="B218" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="B218" s="1" t="s">
+      <c r="C218" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D218" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="E218" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F218" s="1" t="s">
         <v>642</v>
-      </c>
-      <c r="C218" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="D218" s="1" t="s">
-        <v>641</v>
-      </c>
-      <c r="E218" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F218" s="1" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="219" ht="15.75" customHeight="1">
       <c r="A219" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>644</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E219" s="1" t="s">
-        <v>362</v>
+        <v>176</v>
       </c>
       <c r="F219" s="1" t="s">
         <v>645</v>
@@ -7817,27 +7817,27 @@
         <v>646</v>
       </c>
       <c r="B220" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D220" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E220" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F220" s="1" t="s">
         <v>647</v>
-      </c>
-      <c r="C220" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D220" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="E220" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F220" s="1" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="221" ht="15.75" customHeight="1">
       <c r="A221" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>650</v>
@@ -7846,7 +7846,7 @@
         <v>650</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>92</v>
+        <v>351</v>
       </c>
       <c r="F221" s="1" t="s">
         <v>651</v>
@@ -7866,7 +7866,7 @@
         <v>652</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>176</v>
+        <v>92</v>
       </c>
       <c r="F222" s="1" t="s">
         <v>653</v>
@@ -7886,7 +7886,7 @@
         <v>654</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="F223" s="1" t="s">
         <v>655</v>
@@ -7897,27 +7897,27 @@
         <v>656</v>
       </c>
       <c r="B224" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="E224" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F224" s="1" t="s">
         <v>657</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D224" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="E224" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="F224" s="1" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="225" ht="15.75" customHeight="1">
       <c r="A225" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>660</v>
@@ -7926,7 +7926,7 @@
         <v>660</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>74</v>
+        <v>362</v>
       </c>
       <c r="F225" s="1" t="s">
         <v>661</v>
@@ -7937,27 +7937,27 @@
         <v>662</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F226" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="227" ht="15.75" customHeight="1">
       <c r="A227" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>666</v>
@@ -7966,7 +7966,7 @@
         <v>666</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>667</v>
@@ -7986,7 +7986,7 @@
         <v>668</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>220</v>
+        <v>42</v>
       </c>
       <c r="F228" s="1" t="s">
         <v>669</v>
@@ -8006,7 +8006,7 @@
         <v>670</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>45</v>
+        <v>220</v>
       </c>
       <c r="F229" s="1" t="s">
         <v>671</v>
@@ -8017,27 +8017,27 @@
         <v>672</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="E230" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F230" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="231" ht="15.75" customHeight="1">
       <c r="A231" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>676</v>
@@ -8046,7 +8046,7 @@
         <v>676</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>319</v>
+        <v>45</v>
       </c>
       <c r="F231" s="1" t="s">
         <v>677</v>
@@ -8056,48 +8056,48 @@
       <c r="A232" s="1" t="s">
         <v>678</v>
       </c>
-      <c r="B232" s="2" t="s">
+      <c r="B232" s="1" t="s">
         <v>678</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>678</v>
       </c>
       <c r="D232" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="E232" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F232" s="1" t="s">
         <v>679</v>
-      </c>
-      <c r="E232" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="233" ht="15.75" customHeight="1">
       <c r="A233" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D233" s="1" t="s">
         <v>681</v>
       </c>
-      <c r="B233" s="1" t="s">
+      <c r="E233" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F233" s="1" t="s">
         <v>682</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="D233" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="E233" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="F233" s="1" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="234" ht="15.75" customHeight="1">
       <c r="A234" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="C234" s="1" t="s">
         <v>685</v>
@@ -8106,7 +8106,7 @@
         <v>685</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>319</v>
+        <v>362</v>
       </c>
       <c r="F234" s="1" t="s">
         <v>686</v>
@@ -8126,7 +8126,7 @@
         <v>687</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>92</v>
+        <v>319</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>688</v>
@@ -8146,7 +8146,7 @@
         <v>689</v>
       </c>
       <c r="E236" s="1" t="s">
-        <v>319</v>
+        <v>92</v>
       </c>
       <c r="F236" s="1" t="s">
         <v>690</v>
@@ -8157,56 +8157,56 @@
         <v>691</v>
       </c>
       <c r="B237" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D237" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="E237" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F237" s="1" t="s">
         <v>692</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="D237" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="E237" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F237" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="238" ht="15.75" customHeight="1">
       <c r="A238" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>695</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>697</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>695</v>
       </c>
       <c r="E238" s="1" t="s">
-        <v>21</v>
+        <v>255</v>
       </c>
       <c r="F238" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="239" ht="15.75" customHeight="1">
       <c r="A239" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>699</v>
       </c>
-      <c r="D239" s="2" t="s">
-        <v>699</v>
+      <c r="D239" s="1" t="s">
+        <v>697</v>
       </c>
       <c r="E239" s="1" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="F239" s="1" t="s">
         <v>700</v>
@@ -8222,11 +8222,11 @@
       <c r="C240" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="D240" s="1" t="s">
+      <c r="D240" s="2" t="s">
         <v>701</v>
       </c>
       <c r="E240" s="1" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>702</v>
@@ -8246,7 +8246,7 @@
         <v>703</v>
       </c>
       <c r="E241" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="F241" s="1" t="s">
         <v>704</v>
@@ -8266,7 +8266,7 @@
         <v>705</v>
       </c>
       <c r="E242" s="1" t="s">
-        <v>362</v>
+        <v>111</v>
       </c>
       <c r="F242" s="1" t="s">
         <v>706</v>
@@ -8283,30 +8283,30 @@
         <v>707</v>
       </c>
       <c r="D243" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E243" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F243" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="E243" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F243" s="1" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="244" ht="15.75" customHeight="1">
       <c r="A244" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="B244" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D244" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="B244" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="C244" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>710</v>
-      </c>
       <c r="E244" s="1" t="s">
-        <v>141</v>
+        <v>67</v>
       </c>
       <c r="F244" s="1" t="s">
         <v>711</v>
@@ -8326,7 +8326,7 @@
         <v>712</v>
       </c>
       <c r="E245" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="F245" s="1" t="s">
         <v>713</v>
@@ -8346,7 +8346,7 @@
         <v>714</v>
       </c>
       <c r="E246" s="1" t="s">
-        <v>209</v>
+        <v>156</v>
       </c>
       <c r="F246" s="1" t="s">
         <v>715</v>
@@ -8366,7 +8366,7 @@
         <v>716</v>
       </c>
       <c r="E247" s="1" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="F247" s="1" t="s">
         <v>717</v>
@@ -8386,7 +8386,7 @@
         <v>718</v>
       </c>
       <c r="E248" s="1" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="F248" s="1" t="s">
         <v>719</v>
@@ -8406,7 +8406,7 @@
         <v>720</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>141</v>
+        <v>209</v>
       </c>
       <c r="F249" s="1" t="s">
         <v>721</v>
@@ -8416,7 +8416,7 @@
       <c r="A250" s="1" t="s">
         <v>722</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="B250" s="1" t="s">
         <v>722</v>
       </c>
       <c r="C250" s="1" t="s">
@@ -8426,7 +8426,7 @@
         <v>722</v>
       </c>
       <c r="E250" s="1" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="F250" s="1" t="s">
         <v>723</v>
@@ -8436,7 +8436,7 @@
       <c r="A251" s="1" t="s">
         <v>724</v>
       </c>
-      <c r="B251" s="1" t="s">
+      <c r="B251" s="2" t="s">
         <v>724</v>
       </c>
       <c r="C251" s="1" t="s">
@@ -8446,7 +8446,7 @@
         <v>724</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>362</v>
+        <v>176</v>
       </c>
       <c r="F251" s="1" t="s">
         <v>725</v>
@@ -8456,28 +8456,28 @@
       <c r="A252" s="1" t="s">
         <v>726</v>
       </c>
-      <c r="B252" s="2" t="s">
+      <c r="B252" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F252" s="1" t="s">
         <v>727</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="D252" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="E252" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F252" s="1" t="s">
-        <v>729</v>
       </c>
     </row>
     <row r="253" ht="15.75" customHeight="1">
       <c r="A253" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>730</v>
@@ -8486,7 +8486,7 @@
         <v>730</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>148</v>
+        <v>255</v>
       </c>
       <c r="F253" s="1" t="s">
         <v>731</v>
@@ -8500,30 +8500,30 @@
         <v>732</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D254" s="1" t="s">
         <v>732</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>209</v>
+        <v>148</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="255" ht="15.75" customHeight="1">
       <c r="A255" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>734</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>735</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>209</v>
@@ -8536,77 +8536,77 @@
       <c r="A256" s="1" t="s">
         <v>737</v>
       </c>
-      <c r="B256" s="2" t="s">
+      <c r="B256" s="1" t="s">
         <v>737</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D256" s="1" t="s">
         <v>737</v>
       </c>
       <c r="E256" s="1" t="s">
-        <v>319</v>
+        <v>209</v>
       </c>
       <c r="F256" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="257" ht="15.75" customHeight="1">
       <c r="A257" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="C257" s="1" t="s">
         <v>740</v>
       </c>
-      <c r="B257" s="2" t="s">
-        <v>740</v>
-      </c>
-      <c r="C257" s="1" t="s">
+      <c r="D257" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="E257" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F257" s="1" t="s">
         <v>741</v>
-      </c>
-      <c r="D257" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="E257" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F257" s="1" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="258" ht="15.75" customHeight="1">
       <c r="A258" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C258" s="1" t="s">
         <v>743</v>
       </c>
-      <c r="B258" s="2" t="s">
+      <c r="D258" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="E258" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F258" s="1" t="s">
         <v>744</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="D258" s="2" t="s">
-        <v>744</v>
-      </c>
-      <c r="E258" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="F258" s="1" t="s">
-        <v>746</v>
       </c>
     </row>
     <row r="259" ht="15.75" customHeight="1">
       <c r="A259" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>746</v>
       </c>
       <c r="C259" s="1" t="s">
         <v>747</v>
       </c>
-      <c r="D259" s="1" t="s">
-        <v>747</v>
+      <c r="D259" s="2" t="s">
+        <v>746</v>
       </c>
       <c r="E259" s="1" t="s">
-        <v>162</v>
+        <v>269</v>
       </c>
       <c r="F259" s="1" t="s">
         <v>748</v>
@@ -8626,7 +8626,7 @@
         <v>749</v>
       </c>
       <c r="E260" s="1" t="s">
-        <v>319</v>
+        <v>162</v>
       </c>
       <c r="F260" s="1" t="s">
         <v>750</v>
@@ -8637,27 +8637,27 @@
         <v>751</v>
       </c>
       <c r="B261" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D261" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="E261" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F261" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="D261" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="E261" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F261" s="1" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="262" ht="15.75" customHeight="1">
       <c r="A262" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="B262" s="2" t="s">
-        <v>755</v>
+        <v>753</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>754</v>
       </c>
       <c r="C262" s="1" t="s">
         <v>755</v>
@@ -8666,7 +8666,7 @@
         <v>755</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>319</v>
+        <v>11</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>756</v>
@@ -8676,37 +8676,37 @@
       <c r="A263" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="B263" s="1" t="s">
+      <c r="B263" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D263" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="E263" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F263" s="1" t="s">
         <v>758</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="D263" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F263" s="1" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="264" ht="15.75" customHeight="1">
       <c r="A264" s="1" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D264" s="1" t="s">
         <v>762</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>319</v>
+        <v>11</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>763</v>
@@ -8723,30 +8723,30 @@
         <v>764</v>
       </c>
       <c r="D265" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="E265" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F265" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F265" s="1" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="266" ht="15.75" customHeight="1">
       <c r="A266" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D266" s="1" t="s">
         <v>767</v>
       </c>
       <c r="E266" s="1" t="s">
-        <v>111</v>
+        <v>8</v>
       </c>
       <c r="F266" s="1" t="s">
         <v>768</v>
@@ -8766,7 +8766,7 @@
         <v>769</v>
       </c>
       <c r="E267" s="1" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="F267" s="1" t="s">
         <v>770</v>
@@ -8777,7 +8777,7 @@
         <v>771</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C268" s="1" t="s">
         <v>771</v>
@@ -8786,27 +8786,27 @@
         <v>771</v>
       </c>
       <c r="E268" s="1" t="s">
-        <v>245</v>
+        <v>141</v>
       </c>
       <c r="F268" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="269" ht="15.75" customHeight="1">
       <c r="A269" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B269" s="1" t="s">
         <v>774</v>
       </c>
-      <c r="B269" s="2" t="s">
-        <v>774</v>
-      </c>
       <c r="C269" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="E269" s="1" t="s">
-        <v>159</v>
+        <v>245</v>
       </c>
       <c r="F269" s="1" t="s">
         <v>775</v>
@@ -8816,8 +8816,8 @@
       <c r="A270" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="B270" s="1" t="s">
-        <v>777</v>
+      <c r="B270" s="2" t="s">
+        <v>776</v>
       </c>
       <c r="C270" s="1" t="s">
         <v>776</v>
@@ -8826,27 +8826,27 @@
         <v>776</v>
       </c>
       <c r="E270" s="1" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
       <c r="F270" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="271" ht="15.75" customHeight="1">
       <c r="A271" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B271" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="B271" s="2" t="s">
-        <v>779</v>
-      </c>
       <c r="C271" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="E271" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="F271" s="1" t="s">
         <v>780</v>
@@ -8857,27 +8857,27 @@
         <v>781</v>
       </c>
       <c r="B272" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D272" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="E272" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F272" s="1" t="s">
         <v>782</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="D272" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="E272" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F272" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="273" ht="15.75" customHeight="1">
       <c r="A273" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>785</v>
+        <v>783</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>784</v>
       </c>
       <c r="C273" s="1" t="s">
         <v>785</v>
@@ -8886,7 +8886,7 @@
         <v>785</v>
       </c>
       <c r="E273" s="1" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="F273" s="1" t="s">
         <v>786</v>
@@ -8897,27 +8897,27 @@
         <v>787</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="E274" s="1" t="s">
         <v>220</v>
       </c>
       <c r="F274" s="1" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
     </row>
     <row r="275" ht="15.75" customHeight="1">
       <c r="A275" s="1" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="C275" s="1" t="s">
         <v>791</v>
@@ -8926,127 +8926,127 @@
         <v>791</v>
       </c>
       <c r="E275" s="1" t="s">
-        <v>159</v>
+        <v>220</v>
       </c>
       <c r="F275" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="276" ht="15.75" customHeight="1">
       <c r="A276" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="B276" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="B276" s="2" t="s">
+      <c r="C276" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="D276" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="E276" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F276" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="C276" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="D276" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="E276" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F276" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="277" ht="15.75" customHeight="1">
       <c r="A277" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="C277" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="D277" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="B277" s="1" t="s">
+      <c r="E277" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F277" s="1" t="s">
         <v>800</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>799</v>
-      </c>
-      <c r="D277" s="1" t="s">
-        <v>800</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F277" s="1" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="278" ht="15.75" customHeight="1">
       <c r="A278" s="1" t="s">
-        <v>162</v>
+        <v>801</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>162</v>
+        <v>802</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>162</v>
+        <v>801</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>162</v>
+        <v>802</v>
       </c>
       <c r="E278" s="1" t="s">
-        <v>21</v>
+        <v>351</v>
       </c>
       <c r="F278" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
     </row>
     <row r="279" ht="15.75" customHeight="1">
       <c r="A279" s="1" t="s">
-        <v>803</v>
+        <v>162</v>
       </c>
       <c r="B279" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D279" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E279" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F279" s="1" t="s">
         <v>804</v>
-      </c>
-      <c r="C279" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="D279" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="E279" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F279" s="1" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="280" ht="15.75" customHeight="1">
       <c r="A280" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="B280" s="1" t="s">
         <v>806</v>
       </c>
-      <c r="B280" s="1" t="s">
+      <c r="C280" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="D280" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="E280" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F280" s="1" t="s">
         <v>807</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="D280" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="E280" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F280" s="1" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="281" ht="15.75" customHeight="1">
       <c r="A281" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B281" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="B281" s="2" t="s">
-        <v>809</v>
-      </c>
       <c r="C281" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E281" s="1" t="s">
-        <v>42</v>
+        <v>245</v>
       </c>
       <c r="F281" s="1" t="s">
         <v>810</v>
@@ -9056,8 +9056,8 @@
       <c r="A282" s="1" t="s">
         <v>811</v>
       </c>
-      <c r="B282" s="1" t="s">
-        <v>812</v>
+      <c r="B282" s="2" t="s">
+        <v>811</v>
       </c>
       <c r="C282" s="1" t="s">
         <v>811</v>
@@ -9066,1690 +9066,1709 @@
         <v>811</v>
       </c>
       <c r="E282" s="1" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="F282" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="283" ht="15.75" customHeight="1">
       <c r="A283" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="B283" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="B283" s="2" t="s">
+      <c r="C283" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="D283" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="E283" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F283" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="C283" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="D283" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="E283" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F283" s="1" t="s">
+    </row>
+    <row r="284" ht="15.75" customHeight="1">
+      <c r="A284" s="1" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="284" ht="15.75" customHeight="1">
-      <c r="A284" s="2" t="s">
+      <c r="B284" s="2" t="s">
         <v>817</v>
-      </c>
-      <c r="B284" s="2" t="s">
-        <v>818</v>
       </c>
       <c r="C284" s="1" t="s">
         <v>817</v>
       </c>
       <c r="D284" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="E284" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="285" ht="15.75" customHeight="1">
+      <c r="A285" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="B285" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D285" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="E285" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F284" s="1" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="285" ht="15.75" customHeight="1">
-      <c r="A285" s="1" t="s">
+      <c r="F285" s="1" t="s">
         <v>821</v>
-      </c>
-      <c r="B285" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="C285" s="1" t="s">
-        <v>823</v>
-      </c>
-      <c r="D285" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="E285" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F285" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="286" ht="15.75" customHeight="1">
       <c r="A286" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="D286" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="E286" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F286" s="1" t="s">
         <v>825</v>
-      </c>
-      <c r="B286" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>826</v>
-      </c>
-      <c r="D286" s="2" t="s">
-        <v>827</v>
-      </c>
-      <c r="E286" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F286" s="1" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="287" ht="15.75" customHeight="1">
       <c r="A287" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D287" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="E287" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F287" s="1" t="s">
         <v>829</v>
-      </c>
-      <c r="B287" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="C287" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="D287" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="E287" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F287" s="1" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="288" ht="15.75" customHeight="1">
       <c r="A288" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F288" s="1" t="s">
         <v>831</v>
-      </c>
-      <c r="B288" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>833</v>
-      </c>
-      <c r="D288" s="1" t="s">
-        <v>831</v>
-      </c>
-      <c r="E288" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F288" s="1" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="289" ht="15.75" customHeight="1">
       <c r="A289" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="D289" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="E289" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F289" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="B289" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="D289" s="1" t="s">
-        <v>835</v>
-      </c>
-      <c r="E289" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F289" s="1" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="290" ht="15.75" customHeight="1">
       <c r="A290" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="D290" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="E290" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F290" s="1" t="s">
         <v>837</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="D290" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="E290" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="291" ht="15.75" customHeight="1">
       <c r="A291" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="D291" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F291" s="1" t="s">
         <v>839</v>
-      </c>
-      <c r="B291" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="C291" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="D291" s="1" t="s">
-        <v>839</v>
-      </c>
-      <c r="E291" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F291" s="1" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="292" ht="15.75" customHeight="1">
       <c r="A292" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="D292" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F292" s="1" t="s">
         <v>841</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="D292" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F292" s="1" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="293" ht="15.75" customHeight="1">
       <c r="A293" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="D293" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F293" s="1" t="s">
         <v>843</v>
-      </c>
-      <c r="B293" s="1" t="s">
-        <v>844</v>
-      </c>
-      <c r="C293" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="D293" s="2" t="s">
-        <v>846</v>
-      </c>
-      <c r="E293" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F293" s="1" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="294" ht="15.75" customHeight="1">
       <c r="A294" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D294" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="E294" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F294" s="1" t="s">
         <v>848</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>848</v>
-      </c>
-      <c r="C294" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="D294" s="1" t="s">
-        <v>848</v>
-      </c>
-      <c r="E294" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F294" s="1" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="295" ht="15.75" customHeight="1">
       <c r="A295" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>849</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D295" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F295" s="1" t="s">
         <v>850</v>
-      </c>
-      <c r="B295" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="C295" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="D295" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="E295" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F295" s="1" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="296" ht="15.75" customHeight="1">
       <c r="A296" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="D296" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F296" s="1" t="s">
         <v>852</v>
-      </c>
-      <c r="B296" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="C296" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="D296" s="1" t="s">
-        <v>852</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F296" s="1" t="s">
-        <v>853</v>
       </c>
     </row>
     <row r="297" ht="15.75" customHeight="1">
       <c r="A297" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="D297" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F297" s="1" t="s">
         <v>854</v>
-      </c>
-      <c r="B297" s="2" t="s">
-        <v>855</v>
-      </c>
-      <c r="C297" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="D297" s="1" t="s">
-        <v>855</v>
-      </c>
-      <c r="E297" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="F297" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="298" ht="15.75" customHeight="1">
       <c r="A298" s="1" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="E298" s="1" t="s">
         <v>245</v>
       </c>
       <c r="F298" s="1" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
     </row>
     <row r="299" ht="15.75" customHeight="1">
       <c r="A299" s="1" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="E299" s="1" t="s">
         <v>245</v>
       </c>
       <c r="F299" s="1" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="300" ht="15.75" customHeight="1">
       <c r="A300" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="D300" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F300" s="1" t="s">
         <v>864</v>
-      </c>
-      <c r="B300" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="C300" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="D300" s="1" t="s">
-        <v>864</v>
-      </c>
-      <c r="E300" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>865</v>
       </c>
     </row>
     <row r="301" ht="15.75" customHeight="1">
       <c r="A301" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="D301" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F301" s="1" t="s">
         <v>866</v>
-      </c>
-      <c r="B301" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>867</v>
-      </c>
-      <c r="D301" s="1" t="s">
-        <v>866</v>
-      </c>
-      <c r="E301" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F301" s="1" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="302" ht="15.75" customHeight="1">
       <c r="A302" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="B302" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="D302" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F302" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="B302" s="2" t="s">
+    </row>
+    <row r="303" ht="15.75" customHeight="1">
+      <c r="A303" s="2" t="s">
         <v>870</v>
       </c>
-      <c r="C302" s="1" t="s">
+      <c r="B303" s="2" t="s">
         <v>871</v>
       </c>
-      <c r="D302" s="2" t="s">
+      <c r="C303" s="1" t="s">
         <v>872</v>
       </c>
-      <c r="E302" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="F302" s="1" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="303" ht="15.75" customHeight="1">
-      <c r="A303" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="B303" s="2" t="s">
-        <v>875</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>876</v>
-      </c>
       <c r="D303" s="2" t="s">
-        <v>877</v>
+        <v>870</v>
       </c>
       <c r="E303" s="1" t="s">
         <v>351</v>
       </c>
       <c r="F303" s="1" t="s">
-        <v>878</v>
+        <v>873</v>
       </c>
     </row>
     <row r="304" ht="15.75" customHeight="1">
       <c r="A304" s="1" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>880</v>
+        <v>875</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>879</v>
-      </c>
-      <c r="D304" s="1" t="s">
-        <v>879</v>
+        <v>876</v>
+      </c>
+      <c r="D304" s="2" t="s">
+        <v>877</v>
       </c>
       <c r="E304" s="1" t="s">
-        <v>21</v>
+        <v>351</v>
       </c>
       <c r="F304" s="1" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
     </row>
     <row r="305" ht="15.75" customHeight="1">
       <c r="A305" s="1" t="s">
-        <v>882</v>
-      </c>
-      <c r="B305" s="1" t="s">
-        <v>883</v>
+        <v>879</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>880</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>884</v>
+        <v>879</v>
       </c>
       <c r="E305" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F305" s="1" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="306" ht="15.75" customHeight="1">
       <c r="A306" s="1" t="s">
-        <v>886</v>
+        <v>882</v>
       </c>
       <c r="B306" s="1" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="E306" s="1" t="s">
-        <v>74</v>
+        <v>42</v>
       </c>
       <c r="F306" s="1" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="307" ht="15.75" customHeight="1">
       <c r="A307" s="1" t="s">
-        <v>888</v>
-      </c>
-      <c r="B307" s="2" t="s">
-        <v>888</v>
+        <v>886</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>886</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="E307" s="1" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="F307" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
     </row>
     <row r="308" ht="15.75" customHeight="1">
       <c r="A308" s="1" t="s">
-        <v>890</v>
-      </c>
-      <c r="B308" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>888</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E308" s="1" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="F308" s="1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
     <row r="309" ht="15.75" customHeight="1">
       <c r="A309" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B309" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E309" s="1" t="s">
-        <v>138</v>
+        <v>14</v>
       </c>
       <c r="F309" s="1" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="310" ht="15.75" customHeight="1">
       <c r="A310" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B310" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E310" s="1" t="s">
-        <v>42</v>
+        <v>138</v>
       </c>
       <c r="F310" s="1" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="311" ht="15.75" customHeight="1">
       <c r="A311" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="B311" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E311" s="1" t="s">
-        <v>159</v>
+        <v>42</v>
       </c>
       <c r="F311" s="1" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="312" ht="15.75" customHeight="1">
       <c r="A312" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B312" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="E312" s="1" t="s">
         <v>159</v>
       </c>
       <c r="F312" s="1" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="313" ht="15.75" customHeight="1">
       <c r="A313" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B313" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="E313" s="1" t="s">
         <v>159</v>
       </c>
       <c r="F313" s="1" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="314" ht="15.75" customHeight="1">
       <c r="A314" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="B314" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="E314" s="1" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="F314" s="1" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
     </row>
     <row r="315" ht="15.75" customHeight="1">
       <c r="A315" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="B315" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="E315" s="1" t="s">
         <v>120</v>
       </c>
       <c r="F315" s="1" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
     </row>
     <row r="316" ht="15.75" customHeight="1">
       <c r="A316" s="1" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="B316" s="1" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="E316" s="1" t="s">
         <v>120</v>
       </c>
       <c r="F316" s="1" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
     </row>
     <row r="317" ht="15.75" customHeight="1">
       <c r="A317" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="B317" s="1" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="E317" s="1" t="s">
         <v>120</v>
       </c>
       <c r="F317" s="1" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="318" ht="15.75" customHeight="1">
       <c r="A318" s="1" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="B318" s="1" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>914</v>
+        <v>910</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
       <c r="E318" s="1" t="s">
         <v>120</v>
       </c>
       <c r="F318" s="1" t="s">
-        <v>915</v>
+        <v>912</v>
       </c>
     </row>
     <row r="319" ht="15.75" customHeight="1">
       <c r="A319" s="1" t="s">
-        <v>916</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>916</v>
+        <v>913</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>914</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="E319" s="1" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="F319" s="1" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
     </row>
     <row r="320" ht="15.75" customHeight="1">
       <c r="A320" s="1" t="s">
-        <v>919</v>
-      </c>
-      <c r="B320" s="1" t="s">
-        <v>919</v>
+        <v>916</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>916</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="E320" s="1" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="F320" s="1" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="321" ht="15.75" customHeight="1">
       <c r="A321" s="1" t="s">
-        <v>921</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>921</v>
+        <v>919</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>919</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="E321" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F321" s="1" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="322" ht="15.75" customHeight="1">
       <c r="A322" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="E322" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F322" s="1" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="323" ht="15.75" customHeight="1">
       <c r="A323" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="B323" s="1" t="s">
-        <v>926</v>
+        <v>923</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>923</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>925</v>
-      </c>
-      <c r="D323" s="2" t="s">
-        <v>926</v>
+        <v>923</v>
+      </c>
+      <c r="D323" s="1" t="s">
+        <v>923</v>
       </c>
       <c r="E323" s="1" t="s">
-        <v>220</v>
+        <v>29</v>
       </c>
       <c r="F323" s="1" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
     </row>
     <row r="324" ht="15.75" customHeight="1">
       <c r="A324" s="1" t="s">
-        <v>928</v>
-      </c>
-      <c r="B324" s="2" t="s">
-        <v>929</v>
+        <v>925</v>
+      </c>
+      <c r="B324" s="1" t="s">
+        <v>926</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>930</v>
-      </c>
-      <c r="D324" s="1" t="s">
-        <v>928</v>
+        <v>925</v>
+      </c>
+      <c r="D324" s="2" t="s">
+        <v>926</v>
       </c>
       <c r="E324" s="1" t="s">
-        <v>156</v>
+        <v>220</v>
       </c>
       <c r="F324" s="1" t="s">
-        <v>931</v>
+        <v>927</v>
       </c>
     </row>
     <row r="325" ht="15.75" customHeight="1">
       <c r="A325" s="1" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>933</v>
+        <v>929</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>932</v>
+        <v>928</v>
       </c>
       <c r="E325" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F325" s="1" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="326" ht="15.75" customHeight="1">
       <c r="A326" s="1" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>937</v>
+        <v>933</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E326" s="1" t="s">
-        <v>138</v>
+        <v>162</v>
       </c>
       <c r="F326" s="1" t="s">
-        <v>939</v>
+        <v>935</v>
       </c>
     </row>
     <row r="327" ht="15.75" customHeight="1">
       <c r="A327" s="1" t="s">
-        <v>940</v>
-      </c>
-      <c r="B327" s="1" t="s">
-        <v>940</v>
+        <v>936</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>937</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>940</v>
+        <v>936</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>11</v>
+        <v>138</v>
       </c>
       <c r="F327" s="1" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="328" ht="15.75" customHeight="1">
       <c r="A328" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B328" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="F328" s="1" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
     </row>
     <row r="329" ht="15.75" customHeight="1">
       <c r="A329" s="1" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="B329" s="1" t="s">
-        <v>946</v>
+        <v>942</v>
       </c>
       <c r="C329" s="1" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>947</v>
+        <v>942</v>
       </c>
       <c r="E329" s="1" t="s">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="F329" s="1" t="s">
-        <v>948</v>
+        <v>944</v>
       </c>
     </row>
     <row r="330" ht="15.75" customHeight="1">
       <c r="A330" s="1" t="s">
-        <v>949</v>
-      </c>
-      <c r="B330" s="2" t="s">
-        <v>949</v>
+        <v>945</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>946</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="E330" s="1" t="s">
-        <v>8</v>
+        <v>156</v>
       </c>
       <c r="F330" s="1" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
     </row>
     <row r="331" ht="15.75" customHeight="1">
       <c r="A331" s="1" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>953</v>
+        <v>949</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>954</v>
+        <v>950</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="E331" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F331" s="1" t="s">
-        <v>955</v>
+        <v>951</v>
       </c>
     </row>
     <row r="332" ht="15.75" customHeight="1">
       <c r="A332" s="1" t="s">
-        <v>956</v>
-      </c>
-      <c r="B332" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>953</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>956</v>
+        <v>952</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="F332" s="1" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="333" ht="15.75" customHeight="1">
       <c r="A333" s="1" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="B333" s="1" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>960</v>
+        <v>956</v>
       </c>
       <c r="E333" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="F333" s="1" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
     </row>
     <row r="334" ht="15.75" customHeight="1">
       <c r="A334" s="1" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="B334" s="1" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F334" s="1" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
     </row>
     <row r="335" ht="15.75" customHeight="1">
       <c r="A335" s="1" t="s">
-        <v>964</v>
-      </c>
-      <c r="B335" s="2" t="s">
-        <v>964</v>
+        <v>962</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>962</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="E335" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F335" s="1" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
     </row>
     <row r="336" ht="15.75" customHeight="1">
       <c r="A336" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>269</v>
+        <v>8</v>
       </c>
       <c r="F336" s="1" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="337" ht="15.75" customHeight="1">
       <c r="A337" s="1" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>969</v>
-      </c>
-      <c r="D337" s="2" t="s">
-        <v>968</v>
+        <v>966</v>
+      </c>
+      <c r="D337" s="1" t="s">
+        <v>966</v>
       </c>
       <c r="E337" s="1" t="s">
-        <v>159</v>
+        <v>269</v>
       </c>
       <c r="F337" s="1" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
     </row>
     <row r="338" ht="15.75" customHeight="1">
       <c r="A338" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="B338" s="1" t="s">
-        <v>971</v>
+        <v>968</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>968</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="D338" s="1" t="s">
-        <v>971</v>
+        <v>969</v>
+      </c>
+      <c r="D338" s="2" t="s">
+        <v>968</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="F338" s="1" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
     </row>
     <row r="339" ht="15.75" customHeight="1">
       <c r="A339" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="B339" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
     </row>
     <row r="340" ht="15.75" customHeight="1">
       <c r="A340" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="B340" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="E340" s="1" t="s">
-        <v>209</v>
+        <v>17</v>
       </c>
       <c r="F340" s="1" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
     </row>
     <row r="341" ht="15.75" customHeight="1">
       <c r="A341" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="B341" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="E341" s="1" t="s">
-        <v>29</v>
+        <v>209</v>
       </c>
       <c r="F341" s="1" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
     </row>
     <row r="342" ht="15.75" customHeight="1">
       <c r="A342" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="B342" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F342" s="3" t="s">
-        <v>980</v>
+        <v>29</v>
+      </c>
+      <c r="F342" s="1" t="s">
+        <v>978</v>
       </c>
     </row>
     <row r="343" ht="15.75" customHeight="1">
       <c r="A343" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="B343" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="E343" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F343" s="1" t="s">
-        <v>982</v>
+        <v>111</v>
+      </c>
+      <c r="F343" s="3" t="s">
+        <v>980</v>
       </c>
     </row>
     <row r="344" ht="15.75" customHeight="1">
       <c r="A344" s="1" t="s">
-        <v>983</v>
-      </c>
-      <c r="B344" s="2" t="s">
-        <v>983</v>
+        <v>981</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>981</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F344" s="1" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="345" ht="15.75" customHeight="1">
       <c r="A345" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="E345" s="1" t="s">
-        <v>162</v>
+        <v>92</v>
       </c>
       <c r="F345" s="1" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="346" ht="15.75" customHeight="1">
       <c r="A346" s="1" t="s">
-        <v>987</v>
-      </c>
-      <c r="B346" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>985</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
       <c r="F346" s="1" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="347" ht="15.75" customHeight="1">
       <c r="A347" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="B347" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="E347" s="1" t="s">
-        <v>92</v>
+        <v>148</v>
       </c>
       <c r="F347" s="1" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="348" ht="15.75" customHeight="1">
       <c r="A348" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="B348" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F348" s="1" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="349" ht="15.75" customHeight="1">
       <c r="A349" s="1" t="s">
-        <v>993</v>
-      </c>
-      <c r="B349" s="2" t="s">
-        <v>994</v>
+        <v>991</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>991</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="E349" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F349" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
     </row>
     <row r="350" ht="15.75" customHeight="1">
       <c r="A350" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>994</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="E350" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F350" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="351" ht="15.75" customHeight="1">
+      <c r="A351" s="1" t="s">
         <v>997</v>
       </c>
-      <c r="B350" s="1" t="s">
+      <c r="B351" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="C350" s="1" t="s">
+      <c r="C351" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="D350" s="1" t="s">
+      <c r="D351" s="1" t="s">
         <v>999</v>
       </c>
-      <c r="E350" s="1" t="s">
+      <c r="E351" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F350" s="1" t="s">
+      <c r="F351" s="1" t="s">
         <v>1000</v>
       </c>
     </row>
-    <row r="351" ht="15.75" customHeight="1">
-      <c r="A351" s="2" t="s">
+    <row r="352" ht="15.75" customHeight="1">
+      <c r="A352" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="B351" s="2" t="s">
+      <c r="B352" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="D351" s="2" t="s">
+      <c r="D352" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="E351" s="2" t="s">
+      <c r="E352" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="F351" s="3" t="s">
+      <c r="F352" s="3" t="s">
         <v>1004</v>
-      </c>
-    </row>
-    <row r="352" ht="15.75" customHeight="1">
-      <c r="A352" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B352" s="2" t="s">
-        <v>1005</v>
-      </c>
-      <c r="C352" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="D352" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E352" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F352" s="1" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="353" ht="15.75" customHeight="1">
       <c r="A353" s="1" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B353" s="1" t="s">
-        <v>1008</v>
+        <v>1005</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>1005</v>
       </c>
       <c r="C353" s="1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="E353" s="1" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="F353" s="1" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="354" ht="15.75" customHeight="1">
       <c r="A354" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B354" s="1" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>245</v>
+        <v>162</v>
       </c>
       <c r="F354" s="1" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="355" ht="15.75" customHeight="1">
       <c r="A355" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="C355" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="E355" s="1" t="s">
-        <v>269</v>
+        <v>245</v>
       </c>
       <c r="F355" s="1" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="356" ht="15.75" customHeight="1">
       <c r="A356" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>14</v>
+        <v>269</v>
       </c>
       <c r="F356" s="1" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="357" ht="15.75" customHeight="1">
       <c r="A357" s="1" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>1021</v>
+        <v>1016</v>
       </c>
       <c r="E357" s="1" t="s">
-        <v>159</v>
+        <v>14</v>
       </c>
       <c r="F357" s="1" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="358" ht="15.75" customHeight="1">
       <c r="A358" s="1" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B358" s="2" t="s">
-        <v>1023</v>
+        <v>1019</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>1020</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="F358" s="1" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="359" ht="15.75" customHeight="1">
       <c r="A359" s="1" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B359" s="1" t="s">
-        <v>1026</v>
+        <v>1023</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>1023</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="E359" s="1" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
       <c r="F359" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="360" ht="15.75" customHeight="1">
       <c r="A360" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="B360" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>362</v>
+        <v>156</v>
       </c>
       <c r="F360" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="361" ht="15.75" customHeight="1">
       <c r="A361" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="B361" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="E361" s="1" t="s">
-        <v>162</v>
+        <v>362</v>
       </c>
       <c r="F361" s="1" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="362" ht="15.75" customHeight="1">
       <c r="A362" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="B362" s="1" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>1034</v>
+        <v>1030</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="F362" s="1" t="s">
-        <v>1035</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="363" ht="15.75" customHeight="1">
       <c r="A363" s="1" t="s">
-        <v>1036</v>
+        <v>1032</v>
       </c>
       <c r="B363" s="1" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F363" s="3" t="s">
-        <v>1037</v>
+        <v>176</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>1035</v>
       </c>
     </row>
     <row r="364" ht="15.75" customHeight="1">
       <c r="A364" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="B364" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F364" s="1" t="s">
-        <v>1039</v>
+        <v>11</v>
+      </c>
+      <c r="F364" s="3" t="s">
+        <v>1037</v>
       </c>
     </row>
     <row r="365" ht="15.75" customHeight="1">
       <c r="A365" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B365" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="E365" s="1" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F365" s="1" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="366" ht="15.75" customHeight="1">
       <c r="A366" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="E366" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F366" s="1" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="367" ht="15.75" customHeight="1">
+      <c r="A367" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B366" s="2" t="s">
+      <c r="B367" s="2" t="s">
         <v>1043</v>
       </c>
-      <c r="C366" s="1" t="s">
+      <c r="C367" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="D366" s="1" t="s">
+      <c r="D367" s="1" t="s">
         <v>1044</v>
       </c>
-      <c r="E366" s="1" t="s">
+      <c r="E367" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F366" s="1" t="s">
+      <c r="F367" s="1" t="s">
         <v>1045</v>
       </c>
     </row>
-    <row r="367" ht="15.75" customHeight="1"/>
     <row r="368" ht="15.75" customHeight="1"/>
     <row r="369" ht="15.75" customHeight="1"/>
     <row r="370" ht="15.75" customHeight="1"/>
@@ -11386,10 +11405,14 @@
     <row r="1001" ht="15.75" customHeight="1"/>
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
+    <row r="1004" ht="15.75" customHeight="1"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" location="/media/File:New_Haven_Chargers_secondary_logo.svg" ref="F197"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>